<commit_message>
M3 Cord Production System #443 - M3.Cord.Production.App re-implements #243.
</commit_message>
<xml_diff>
--- a/Documents/Cord/Cord Documents/4007 of RF-TW-14-04  Ageing Condition (S-5).xlsx
+++ b/Documents/Cord/Cord Documents/4007 of RF-TW-14-04  Ageing Condition (S-5).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15600" windowHeight="7680"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="15600" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="P1671TT " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -390,7 +390,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="187" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1406,13 +1406,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="187" fontId="10" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="10" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1558,6 +1558,189 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1573,12 +1756,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1609,188 +1786,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
     <cellStyle name="ปกติ_Original" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2885,7 +2885,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ชุดรูปแบบของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3171,33 +3171,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="95" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="95" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" thickBot="1"/>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="30" thickTop="1">
-      <c r="A2" s="131" t="s">
+    <row r="1" spans="1:9" ht="21.6" thickBot="1"/>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="29.4" thickTop="1">
+      <c r="A2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="132"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3209,86 +3209,86 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="F3" s="6">
         <f ca="1">TODAY()</f>
-        <v>44166</v>
+        <v>45124</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A4" s="133"/>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
     </row>
     <row r="5" spans="1:9" ht="33" customHeight="1">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="135" t="s">
+      <c r="B5" s="113"/>
+      <c r="C5" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="136"/>
+      <c r="D5" s="114"/>
       <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="135" t="s">
+      <c r="G5" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="136"/>
+      <c r="H5" s="114"/>
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="33" customHeight="1">
-      <c r="A6" s="137" t="s">
+      <c r="A6" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="134"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="139"/>
-      <c r="G6" s="135" t="s">
+      <c r="F6" s="117"/>
+      <c r="G6" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="136"/>
+      <c r="H6" s="114"/>
     </row>
     <row r="7" spans="1:9" ht="33" customHeight="1">
-      <c r="A7" s="140" t="s">
+      <c r="A7" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="15"/>
-      <c r="E7" s="142" t="s">
+      <c r="E7" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="143"/>
+      <c r="F7" s="121"/>
       <c r="G7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="24">
+    <row r="8" spans="1:9" ht="24.6">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="17"/>
@@ -3298,11 +3298,11 @@
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="30" thickBot="1">
-      <c r="A9" s="130" t="s">
+    <row r="9" spans="1:9" ht="29.4" thickBot="1">
+      <c r="A9" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="130"/>
+      <c r="B9" s="108"/>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
@@ -3322,46 +3322,46 @@
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" ht="29.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="122" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="116" t="s">
+      <c r="B10" s="123"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="117"/>
-      <c r="G10" s="118" t="s">
+      <c r="F10" s="125"/>
+      <c r="G10" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="119"/>
+      <c r="H10" s="127"/>
     </row>
     <row r="11" spans="1:9" s="24" customFormat="1" ht="19.5" customHeight="1" thickTop="1">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="126" t="s">
+      <c r="C11" s="131"/>
+      <c r="D11" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="97"/>
-      <c r="G11" s="128" t="s">
+      <c r="F11" s="137"/>
+      <c r="G11" s="138" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="129"/>
+      <c r="H11" s="139"/>
     </row>
-    <row r="12" spans="1:9" s="24" customFormat="1" ht="24">
-      <c r="A12" s="121"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="127"/>
+    <row r="12" spans="1:9" s="24" customFormat="1" ht="24.6">
+      <c r="A12" s="129"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="135"/>
       <c r="E12" s="25" t="s">
         <v>30</v>
       </c>
@@ -3379,10 +3379,10 @@
       <c r="A13" s="29">
         <v>1</v>
       </c>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="111"/>
+      <c r="C13" s="143"/>
       <c r="D13" s="30"/>
       <c r="E13" s="31" t="s">
         <v>35</v>
@@ -3397,10 +3397,10 @@
       <c r="A14" s="29">
         <v>2</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="111"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="30"/>
       <c r="E14" s="31" t="s">
         <v>35</v>
@@ -3415,10 +3415,10 @@
       <c r="A15" s="35">
         <v>3</v>
       </c>
-      <c r="B15" s="110" t="s">
+      <c r="B15" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="112"/>
+      <c r="C15" s="144"/>
       <c r="D15" s="36"/>
       <c r="E15" s="37" t="s">
         <v>38</v>
@@ -3433,10 +3433,10 @@
       <c r="A16" s="35">
         <v>4</v>
       </c>
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="142" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="112"/>
+      <c r="C16" s="144"/>
       <c r="D16" s="36"/>
       <c r="E16" s="37" t="s">
         <v>40</v>
@@ -3469,10 +3469,10 @@
       <c r="A18" s="40">
         <v>6</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="113"/>
+      <c r="C18" s="145"/>
       <c r="D18" s="43"/>
       <c r="E18" s="46" t="s">
         <v>44</v>
@@ -3487,39 +3487,39 @@
       <c r="A19" s="50">
         <v>7</v>
       </c>
-      <c r="B19" s="144" t="s">
+      <c r="B19" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="145"/>
-      <c r="D19" s="146" t="s">
+      <c r="C19" s="147"/>
+      <c r="D19" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="147" t="s">
+      <c r="E19" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="148"/>
-      <c r="G19" s="149" t="s">
+      <c r="F19" s="93"/>
+      <c r="G19" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="150"/>
+      <c r="H19" s="95"/>
     </row>
     <row r="20" spans="1:12" s="51" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="35">
         <v>8</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="152"/>
-      <c r="D20" s="153"/>
-      <c r="E20" s="154" t="s">
+      <c r="C20" s="149"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="153"/>
-      <c r="G20" s="155" t="s">
+      <c r="F20" s="96"/>
+      <c r="G20" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="156"/>
+      <c r="H20" s="99"/>
       <c r="L20" s="51" t="s">
         <v>51</v>
       </c>
@@ -3528,59 +3528,59 @@
       <c r="A21" s="50">
         <v>9</v>
       </c>
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="148" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="152"/>
-      <c r="D21" s="157" t="s">
+      <c r="C21" s="149"/>
+      <c r="D21" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="154" t="s">
+      <c r="E21" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="153"/>
-      <c r="G21" s="155" t="s">
+      <c r="F21" s="96"/>
+      <c r="G21" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="156"/>
+      <c r="H21" s="99"/>
     </row>
     <row r="22" spans="1:12" s="51" customFormat="1" ht="34.5" customHeight="1">
       <c r="A22" s="35">
         <v>10</v>
       </c>
-      <c r="B22" s="158" t="s">
+      <c r="B22" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="159"/>
-      <c r="D22" s="160"/>
-      <c r="E22" s="161" t="s">
+      <c r="C22" s="151"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="160"/>
-      <c r="G22" s="162" t="s">
+      <c r="F22" s="101"/>
+      <c r="G22" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="163"/>
+      <c r="H22" s="104"/>
     </row>
     <row r="23" spans="1:12" s="51" customFormat="1" ht="48" customHeight="1">
       <c r="A23" s="50">
         <v>11</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="109"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="36"/>
-      <c r="E23" s="164" t="s">
+      <c r="E23" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="165" t="s">
+      <c r="F23" s="106" t="s">
         <v>82</v>
       </c>
       <c r="G23" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="166">
+      <c r="H23" s="107">
         <v>14.4</v>
       </c>
     </row>
@@ -3588,10 +3588,10 @@
       <c r="A24" s="35">
         <v>12</v>
       </c>
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="109"/>
+      <c r="C24" s="141"/>
       <c r="D24" s="36"/>
       <c r="E24" s="54" t="s">
         <v>60</v>
@@ -3606,10 +3606,10 @@
       <c r="A25" s="50">
         <v>13</v>
       </c>
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="109"/>
+      <c r="C25" s="141"/>
       <c r="D25" s="36"/>
       <c r="E25" s="54" t="s">
         <v>60</v>
@@ -3644,10 +3644,10 @@
       <c r="A27" s="63">
         <v>15</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="95"/>
+      <c r="C27" s="156"/>
       <c r="D27" s="64"/>
       <c r="E27" s="65" t="s">
         <v>68</v>
@@ -3660,21 +3660,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="51" customFormat="1" ht="19.5" thickTop="1">
+    <row r="28" spans="1:12" s="51" customFormat="1" ht="19.2" thickTop="1">
       <c r="A28" s="68" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="69"/>
       <c r="C28" s="69"/>
       <c r="D28" s="70"/>
-      <c r="E28" s="96" t="s">
+      <c r="E28" s="136" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="97"/>
-      <c r="G28" s="98" t="s">
+      <c r="F28" s="137"/>
+      <c r="G28" s="157" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="99"/>
+      <c r="H28" s="158"/>
     </row>
     <row r="29" spans="1:12" s="73" customFormat="1">
       <c r="A29" s="71" t="s">
@@ -3683,14 +3683,14 @@
       <c r="B29" s="72"/>
       <c r="C29" s="72"/>
       <c r="D29" s="72"/>
-      <c r="E29" s="100" t="s">
+      <c r="E29" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="101"/>
-      <c r="G29" s="102" t="s">
+      <c r="F29" s="160"/>
+      <c r="G29" s="161" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="103"/>
+      <c r="H29" s="162"/>
     </row>
     <row r="30" spans="1:12" s="73" customFormat="1" ht="51" customHeight="1" thickBot="1">
       <c r="A30" s="71" t="s">
@@ -3722,14 +3722,14 @@
       <c r="B32" s="72"/>
       <c r="C32" s="72"/>
       <c r="D32" s="72"/>
-      <c r="E32" s="104" t="s">
+      <c r="E32" s="163" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="105"/>
-      <c r="G32" s="106" t="s">
+      <c r="F32" s="164"/>
+      <c r="G32" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="H32" s="107"/>
+      <c r="H32" s="166"/>
     </row>
     <row r="33" spans="1:9" s="73" customFormat="1">
       <c r="A33" s="71"/>
@@ -3751,15 +3751,15 @@
       <c r="G34" s="88"/>
       <c r="H34" s="89"/>
     </row>
-    <row r="35" spans="1:9" s="73" customFormat="1" ht="23.25" thickTop="1" thickBot="1">
+    <row r="35" spans="1:9" s="73" customFormat="1" ht="22.2" thickTop="1" thickBot="1">
       <c r="A35" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="91" t="s">
+      <c r="F35" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="G35" s="92"/>
-      <c r="H35" s="93"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="154"/>
     </row>
     <row r="36" spans="1:9" s="73" customFormat="1">
       <c r="A36" s="1"/>
@@ -3776,6 +3776,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -3788,34 +3816,6 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>